<commit_message>
update automation testing registration page
</commit_message>
<xml_diff>
--- a/registration_TC.xlsx
+++ b/registration_TC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\WC3-Homework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41DF238C-62EE-4F8F-90DE-26D9E6A124CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{701DD907-E4FC-437E-9CE8-9C8678FA47AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D5C06684-A1C2-4990-A084-4BB9B2236277}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D5C06684-A1C2-4990-A084-4BB9B2236277}"/>
   </bookViews>
   <sheets>
     <sheet name="Demo QA - Registration form" sheetId="2" r:id="rId1"/>
@@ -363,11 +363,6 @@
     <t>TCRegister#12</t>
   </si>
   <si>
-    <t>Verify that user submit successfully when first name, last name, current adrress have abundant space  at the begin and end of input data:
-- First name, Last name, Current Adress have more than 255 characters.
-- Picture file's size exceeds limit file size 2MB.</t>
-  </si>
-  <si>
     <t>First Name:"  Lam  "
 Last Name: "  Tran  "
 Gender: Female
@@ -385,6 +380,9 @@
   </si>
   <si>
     <t>Usert cannot submit</t>
+  </si>
+  <si>
+    <t>Verify that user submit successfully when first name, last name, current adrress have abundant space  at the begin and end of input data</t>
   </si>
 </sst>
 </file>
@@ -811,13 +809,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>5006698</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>854075</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -855,14 +853,14 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2662757</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>2441448</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1107948</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1234,6 +1232,45 @@
         <a:xfrm>
           <a:off x="17191182" y="28609636"/>
           <a:ext cx="1743363" cy="1606799"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2662757" cy="2441448"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C38EFE3-0F47-47A3-8A21-754F5C12E65A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19278600" y="14582775"/>
+          <a:ext cx="2662757" cy="2441448"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1544,27 +1581,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FD9765C-88F0-4954-8592-D53FEDCC6EDF}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="53" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="G1" activePane="topRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="topRight" activeCell="C14" sqref="C14"/>
+      <selection pane="topRight" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="18.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="66.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="56.54296875" customWidth="1"/>
-    <col min="7" max="7" width="70.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="88.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.1796875" style="25"/>
-    <col min="10" max="10" width="75.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56.5703125" customWidth="1"/>
+    <col min="7" max="7" width="70.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="88.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="25"/>
+    <col min="10" max="10" width="75.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
         <v>8</v>
       </c>
@@ -1578,12 +1615,12 @@
       <c r="I1" s="15"/>
       <c r="J1" s="24"/>
     </row>
-    <row r="2" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>1</v>
@@ -1610,12 +1647,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="203" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>60</v>
@@ -1638,7 +1675,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="153.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="153.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
@@ -1662,23 +1699,23 @@
       </c>
       <c r="J4" s="24"/>
     </row>
-    <row r="5" spans="1:10" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="32"/>
       <c r="C5" s="8" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="7" t="s">
         <v>57</v>
       </c>
       <c r="F5" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>64</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>65</v>
       </c>
       <c r="H5" s="20"/>
       <c r="I5" s="16" t="s">
@@ -1686,12 +1723,12 @@
       </c>
       <c r="J5" s="24"/>
     </row>
-    <row r="6" spans="1:10" ht="101.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="101.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>38</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>25</v>
@@ -1710,7 +1747,7 @@
       </c>
       <c r="J6" s="24"/>
     </row>
-    <row r="7" spans="1:10" ht="203.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="203.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>39</v>
       </c>
@@ -1734,55 +1771,55 @@
       </c>
       <c r="J7" s="24"/>
     </row>
-    <row r="8" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="202.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>40</v>
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="14" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="H8" s="22"/>
-      <c r="I8" s="16" t="s">
-        <v>13</v>
+        <v>41</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="21"/>
+      <c r="I8" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="J8" s="24"/>
     </row>
-    <row r="9" spans="1:10" ht="202.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="14" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="13" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" s="21"/>
-      <c r="I9" s="17" t="s">
-        <v>15</v>
+        <v>47</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="22"/>
+      <c r="I9" s="16" t="s">
+        <v>13</v>
       </c>
       <c r="J9" s="24"/>
     </row>
-    <row r="10" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>20</v>
       </c>
@@ -1806,7 +1843,7 @@
       </c>
       <c r="J10" s="24"/>
     </row>
-    <row r="11" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>21</v>
       </c>
@@ -1830,7 +1867,7 @@
       </c>
       <c r="J11" s="24"/>
     </row>
-    <row r="12" spans="1:10" ht="205.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="205.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>49</v>
       </c>
@@ -1854,7 +1891,7 @@
       </c>
       <c r="J12" s="24"/>
     </row>
-    <row r="13" spans="1:10" ht="319" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="330" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>55</v>
       </c>
@@ -1880,7 +1917,7 @@
       </c>
       <c r="J13" s="24"/>
     </row>
-    <row r="14" spans="1:10" ht="362.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="375" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>62</v>
       </c>
@@ -1904,56 +1941,56 @@
       </c>
       <c r="J14" s="24"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="3"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="3"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="3"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="3"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="3"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="3"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="3"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="3"/>

</xml_diff>